<commit_message>
bán hàng. hóa đơn, thống kê
</commit_message>
<xml_diff>
--- a/src/Excel/Bill_Excel/B3.xlsx
+++ b/src/Excel/Bill_Excel/B3.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="24">
   <si>
     <t/>
   </si>
@@ -29,7 +29,7 @@
     <t>Ngày:</t>
   </si>
   <si>
-    <t>2022-12-07 19:12:00</t>
+    <t>2023-11-29 17:46:50</t>
   </si>
   <si>
     <t>Staff:</t>
@@ -38,6 +38,12 @@
     <t>Nguyễn Ngọc Trường Chinh</t>
   </si>
   <si>
+    <t>Khách:</t>
+  </si>
+  <si>
+    <t>w6Cfy19ejrOSkW3NkazDfOeduDNzhrmgTdpglJOLc9M=</t>
+  </si>
+  <si>
     <t>------------------------------------------------------------------------------------------------------------------------------------------------</t>
   </si>
   <si>
@@ -59,40 +65,25 @@
     <t>Thành tiền</t>
   </si>
   <si>
-    <t>Hamburger gà sốt BBQ (4 oz)</t>
-  </si>
-  <si>
-    <t>40.000 ₫</t>
-  </si>
-  <si>
-    <t>34.000 ₫</t>
-  </si>
-  <si>
-    <t>68.000 ₫</t>
-  </si>
-  <si>
-    <t>Bít tết đặc biệt (Nhỏ)</t>
-  </si>
-  <si>
-    <t>90.000 ₫</t>
+    <t>Gà nướng muối ớt (1 con)</t>
+  </si>
+  <si>
+    <t>130.000 ₫</t>
   </si>
   <si>
     <t>Tổng:</t>
   </si>
   <si>
-    <t>158.000 ₫</t>
-  </si>
-  <si>
     <t>Tiền nhận:</t>
   </si>
   <si>
-    <t>1.111.111 ₫</t>
+    <t>200.000 ₫</t>
   </si>
   <si>
     <t>Tiền thối:</t>
   </si>
   <si>
-    <t>-953.111 ₫</t>
+    <t>-70.000 ₫</t>
   </si>
 </sst>
 </file>
@@ -632,7 +623,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:L19"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -684,6 +675,12 @@
       <c r="B5" t="s" s="4">
         <v>7</v>
       </c>
+      <c r="H5" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="I5" t="s" s="4">
+        <v>9</v>
+      </c>
       <c r="L5" s="5"/>
     </row>
     <row r="6">
@@ -693,7 +690,7 @@
     <row r="7">
       <c r="A7" s="6"/>
       <c r="B7" t="s" s="2">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="L7" s="5"/>
     </row>
@@ -703,22 +700,22 @@
     </row>
     <row r="9">
       <c r="A9" t="s" s="8">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s" s="2">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F9" t="s" s="2">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G9" t="s" s="2">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="I9" t="s" s="2">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="K9" t="s" s="2">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="L9" s="5"/>
     </row>
@@ -731,16 +728,13 @@
         <v>1.0</v>
       </c>
       <c r="B11" t="s" s="4">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F11" t="n" s="4">
-        <v>2.0</v>
-      </c>
-      <c r="G11" t="s" s="3">
-        <v>16</v>
-      </c>
-      <c r="I11" t="s" s="4">
-        <v>17</v>
+        <v>1.0</v>
+      </c>
+      <c r="G11" t="s" s="4">
+        <v>18</v>
       </c>
       <c r="K11" t="s" s="4">
         <v>18</v>
@@ -748,88 +742,71 @@
       <c r="L11" s="5"/>
     </row>
     <row r="12">
-      <c r="A12" t="n" s="9">
-        <v>2.0</v>
-      </c>
-      <c r="B12" t="s" s="4">
-        <v>19</v>
-      </c>
-      <c r="F12" t="n" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="G12" t="s" s="4">
-        <v>20</v>
-      </c>
-      <c r="K12" t="s" s="4">
-        <v>20</v>
-      </c>
+      <c r="A12" s="6"/>
       <c r="L12" s="5"/>
     </row>
     <row r="13">
       <c r="A13" s="6"/>
+      <c r="B13" t="s" s="2">
+        <v>10</v>
+      </c>
       <c r="L13" s="5"/>
     </row>
     <row r="14">
       <c r="A14" s="6"/>
-      <c r="B14" t="s" s="2">
-        <v>8</v>
-      </c>
       <c r="L14" s="5"/>
     </row>
     <row r="15">
       <c r="A15" s="6"/>
+      <c r="G15" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="I15" t="s" s="4">
+        <v>18</v>
+      </c>
       <c r="L15" s="5"/>
     </row>
     <row r="16">
       <c r="A16" s="6"/>
       <c r="G16" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="I16" t="s" s="4">
         <v>21</v>
-      </c>
-      <c r="I16" t="s" s="4">
-        <v>22</v>
       </c>
       <c r="L16" s="5"/>
     </row>
     <row r="17">
       <c r="A17" s="6"/>
       <c r="G17" t="s" s="2">
+        <v>22</v>
+      </c>
+      <c r="I17" t="s" s="4">
         <v>23</v>
       </c>
-      <c r="I17" t="s" s="4">
-        <v>24</v>
-      </c>
       <c r="L17" s="5"/>
     </row>
     <row r="18">
-      <c r="A18" s="6"/>
-      <c r="G18" t="s" s="2">
-        <v>25</v>
-      </c>
-      <c r="I18" t="s" s="4">
-        <v>26</v>
-      </c>
-      <c r="L18" s="5"/>
-    </row>
-    <row r="19">
-      <c r="A19" s="13"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="14"/>
-      <c r="L19" s="15"/>
+      <c r="A18" s="13"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="24">
+  <mergeCells count="21">
     <mergeCell ref="A2:L2"/>
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="I4:L4"/>
     <mergeCell ref="B5:E5"/>
+    <mergeCell ref="I5:L5"/>
     <mergeCell ref="B7:K7"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="G9:H9"/>
@@ -839,17 +816,13 @@
     <mergeCell ref="G11:H11"/>
     <mergeCell ref="I11:J11"/>
     <mergeCell ref="K11:L11"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="B14:K14"/>
+    <mergeCell ref="B13:K13"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="I15:K15"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="I16:K16"/>
     <mergeCell ref="G17:H17"/>
     <mergeCell ref="I17:K17"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="I18:K18"/>
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>